<commit_message>
Dispertion curve plots on GUI, added option to plot dispertion curve on a external window
</commit_message>
<xml_diff>
--- a/example/example_dispertion1.xlsx
+++ b/example/example_dispertion1.xlsx
@@ -37,7 +37,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -73,7 +73,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>